<commit_message>
Updated dcp2T1 with Amnon's notebook
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1525,7 +1525,7 @@
       <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr"/>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr"/>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W7" t="inlineStr"/>
@@ -1649,7 +1649,7 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr"/>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr"/>
@@ -1765,7 +1765,7 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W8" t="inlineStr"/>
@@ -1773,7 +1773,7 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr"/>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W9" t="inlineStr"/>
@@ -1897,7 +1897,7 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr"/>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr"/>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W10" t="inlineStr"/>
@@ -2021,7 +2021,7 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr"/>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="AF10" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG10" t="inlineStr"/>
@@ -2145,7 +2145,7 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr"/>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W12" t="inlineStr"/>
@@ -2269,7 +2269,7 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr"/>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="AF12" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG12" t="inlineStr"/>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W13" t="inlineStr"/>
@@ -2393,7 +2393,7 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA13" t="inlineStr"/>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr"/>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W14" t="inlineStr"/>
@@ -2517,7 +2517,7 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA14" t="inlineStr"/>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr"/>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W15" t="inlineStr"/>
@@ -2641,7 +2641,7 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr"/>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr"/>
@@ -2765,7 +2765,7 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA16" t="inlineStr"/>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr"/>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W17" t="inlineStr"/>
@@ -2889,7 +2889,7 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA17" t="inlineStr"/>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W18" t="inlineStr"/>
@@ -3013,7 +3013,7 @@
       <c r="Y18" t="inlineStr"/>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA18" t="inlineStr"/>
@@ -3035,7 +3035,7 @@
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr"/>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W19" t="inlineStr"/>
@@ -3137,7 +3137,7 @@
       <c r="Y19" t="inlineStr"/>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA19" t="inlineStr"/>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="AF19" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG19" t="inlineStr"/>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W20" t="inlineStr"/>
@@ -3261,7 +3261,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA20" t="inlineStr"/>
@@ -3283,7 +3283,7 @@
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr"/>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W21" t="inlineStr"/>
@@ -3385,7 +3385,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA21" t="inlineStr"/>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr"/>
@@ -3509,7 +3509,7 @@
       <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA22" t="inlineStr"/>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr"/>
@@ -3625,7 +3625,7 @@
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W23" t="inlineStr"/>
@@ -3633,7 +3633,7 @@
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA23" t="inlineStr"/>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG23" t="inlineStr"/>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W24" t="inlineStr"/>
@@ -3757,7 +3757,7 @@
       <c r="Y24" t="inlineStr"/>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA24" t="inlineStr"/>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="AF24" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG24" t="inlineStr"/>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W25" t="inlineStr"/>
@@ -3881,7 +3881,7 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA25" t="inlineStr"/>
@@ -3903,7 +3903,7 @@
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr"/>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="V26" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W26" t="inlineStr"/>
@@ -4005,7 +4005,7 @@
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA26" t="inlineStr"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr"/>
@@ -4121,7 +4121,7 @@
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W27" t="inlineStr"/>
@@ -4129,7 +4129,7 @@
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA27" t="inlineStr"/>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr"/>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W28" t="inlineStr"/>
@@ -4253,7 +4253,7 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA28" t="inlineStr"/>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="AF28" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG28" t="inlineStr"/>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W29" t="inlineStr"/>
@@ -4377,7 +4377,7 @@
       <c r="Y29" t="inlineStr"/>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA29" t="inlineStr"/>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="AF29" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG29" t="inlineStr"/>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W30" t="inlineStr"/>
@@ -4501,7 +4501,7 @@
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA30" t="inlineStr"/>
@@ -4523,7 +4523,7 @@
       </c>
       <c r="AF30" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG30" t="inlineStr"/>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W31" t="inlineStr"/>
@@ -4625,7 +4625,7 @@
       <c r="Y31" t="inlineStr"/>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA31" t="inlineStr"/>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="AF31" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG31" t="inlineStr"/>
@@ -4741,7 +4741,7 @@
       </c>
       <c r="V32" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W32" t="inlineStr"/>
@@ -4749,7 +4749,7 @@
       <c r="Y32" t="inlineStr"/>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA32" t="inlineStr"/>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="AF32" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG32" t="inlineStr"/>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W33" t="inlineStr"/>
@@ -4873,7 +4873,7 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA33" t="inlineStr"/>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="AF33" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG33" t="inlineStr"/>
@@ -4989,7 +4989,7 @@
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>na</t>
+          <t>DAPI-||nan</t>
         </is>
       </c>
       <c r="W34" t="inlineStr"/>
@@ -4997,7 +4997,7 @@
       <c r="Y34" t="inlineStr"/>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>EFO:0009900</t>
+          <t>EFO:0009900||EFO:0010714</t>
         </is>
       </c>
       <c r="AA34" t="inlineStr"/>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="AF34" t="inlineStr">
         <is>
-          <t>GRCh37</t>
+          <t>GRCh37||GRCh38</t>
         </is>
       </c>
       <c r="AG34" t="inlineStr"/>

</xml_diff>

<commit_message>
Added more automatic conversions to dcp2T1 notebook
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1467,10 +1467,14 @@
           <t>PBMCs</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>PBMCs</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
@@ -1591,10 +1595,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
@@ -1715,10 +1723,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
@@ -1839,10 +1851,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
@@ -1963,10 +1979,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
@@ -2087,10 +2107,14 @@
           <t>PBMCs</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>PBMCs</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
@@ -2211,10 +2235,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
@@ -2335,10 +2363,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
@@ -2459,10 +2491,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
@@ -2583,10 +2619,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L15" t="inlineStr"/>
@@ -2707,10 +2747,14 @@
           <t>PBMCs</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>PBMCs</t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L16" t="inlineStr"/>
@@ -2831,10 +2875,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
@@ -2955,10 +3003,14 @@
           <t>Cell suspension from lymph node</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Cell suspension from lymph node</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L18" t="inlineStr"/>
@@ -3079,10 +3131,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L19" t="inlineStr"/>
@@ -3203,10 +3259,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L20" t="inlineStr"/>
@@ -3327,10 +3387,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L21" t="inlineStr"/>
@@ -3451,10 +3515,14 @@
           <t>PBMCs</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>PBMCs</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L22" t="inlineStr"/>
@@ -3575,10 +3643,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L23" t="inlineStr"/>
@@ -3699,10 +3771,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr"/>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L24" t="inlineStr"/>
@@ -3823,10 +3899,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr"/>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L25" t="inlineStr"/>
@@ -3947,10 +4027,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L26" t="inlineStr"/>
@@ -4071,10 +4155,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L27" t="inlineStr"/>
@@ -4195,10 +4283,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr"/>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L28" t="inlineStr"/>
@@ -4319,10 +4411,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr"/>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L29" t="inlineStr"/>
@@ -4443,10 +4539,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr"/>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L30" t="inlineStr"/>
@@ -4567,10 +4667,14 @@
           <t>Cell suspension from normal kidney tissue</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Cell suspension from normal kidney tissue</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L31" t="inlineStr"/>
@@ -4691,10 +4795,14 @@
           <t>Cell suspension from tumor tissue (Center)</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Center)</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L32" t="inlineStr"/>
@@ -4815,10 +4923,14 @@
           <t>Cell suspension from tumor tissue (Far)</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr"/>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Far)</t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L33" t="inlineStr"/>
@@ -4939,10 +5051,14 @@
           <t>Cell suspension from tumor tissue (Near)</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Cell suspension from tumor tissue (Near)</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>9606</t>
+          <t>NCBITaxon:9606</t>
         </is>
       </c>
       <c r="L34" t="inlineStr"/>

</xml_diff>

<commit_message>
Populate tier1 fields not filled in export spreadsheet
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -633,7 +633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL34"/>
+  <dimension ref="A1:AN34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -832,6 +832,16 @@
           <t>development_stage_ontology_term_id</t>
         </is>
       </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>author_cell_type</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>cell_type_ontology_term_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1036,6 +1046,8 @@
 </t>
         </is>
       </c>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1210,6 +1222,8 @@
 </t>
         </is>
       </c>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1400,6 +1414,8 @@
           <t>HsapDv:0000237; unknown</t>
         </is>
       </c>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1444,10 +1460,16 @@
       <c r="AJ5" t="inlineStr"/>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_PBMC</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1572,10 +1594,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_kidney</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1700,10 +1728,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Center</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1828,10 +1862,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Far</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1956,10 +1996,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Near</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -2084,10 +2130,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_PBMC</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2212,10 +2264,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_kidney</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2340,10 +2398,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Center</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2468,10 +2532,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Far</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2596,10 +2666,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Near</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2724,10 +2800,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_PBMC</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -2852,10 +2934,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_kidney</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -2980,10 +3068,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_lymph_node</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3108,10 +3202,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Center</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3236,10 +3336,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Far</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3364,10 +3470,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Near</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3492,10 +3604,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NivoExposed_PBMC</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3620,10 +3738,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NivoExposed_kidney</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3748,10 +3872,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Center</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3876,10 +4006,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Far</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4004,10 +4140,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Near</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4132,10 +4274,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>UT1_kidney</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4260,10 +4408,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Center</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4388,10 +4542,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Far</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4516,10 +4676,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Near</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4644,10 +4810,16 @@
           <t>HsapDv:0000241</t>
         </is>
       </c>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>UT2_kidney</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -4772,10 +4944,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Center</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -4900,10 +5078,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Far</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -5028,10 +5212,16 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Near</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -5156,6 +5346,8 @@
           <t>HsapDv:0000240</t>
         </is>
       </c>
+      <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Remove duplication of sample_id column in dcp2T1
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1465,11 +1465,7 @@
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>IpiNivo_Complete_PBMC</t>
-        </is>
-      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1599,11 +1595,7 @@
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>IpiNivo_Complete_kidney</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1733,11 +1725,7 @@
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>IpiNivo_Complete_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1867,11 +1855,7 @@
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>IpiNivo_Complete_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -2001,11 +1985,7 @@
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>IpiNivo_Complete_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -2135,11 +2115,7 @@
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>IpiNivo_Mixed_PBMC</t>
-        </is>
-      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2269,11 +2245,7 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>IpiNivo_Mixed_kidney</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2403,11 +2375,7 @@
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>IpiNivo_Mixed_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2537,11 +2505,7 @@
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>IpiNivo_Mixed_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2671,11 +2635,7 @@
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>IpiNivo_Mixed_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2805,11 +2765,7 @@
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_PBMC</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -2939,11 +2895,7 @@
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_kidney</t>
-        </is>
-      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3073,11 +3025,7 @@
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_lymph_node</t>
-        </is>
-      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3207,11 +3155,7 @@
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3341,11 +3285,7 @@
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3475,11 +3415,7 @@
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>IpiNivo_Resistant_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3609,11 +3545,7 @@
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>NivoExposed_PBMC</t>
-        </is>
-      </c>
+      <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3743,11 +3675,7 @@
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>NivoExposed_kidney</t>
-        </is>
-      </c>
+      <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3877,11 +3805,7 @@
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>NivoExposed_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4011,11 +3935,7 @@
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>NivoExposed_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4145,11 +4065,7 @@
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>NivoExposed_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4279,11 +4195,7 @@
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>UT1_kidney</t>
-        </is>
-      </c>
+      <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4413,11 +4325,7 @@
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>UT1_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4547,11 +4455,7 @@
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>UT1_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4681,11 +4585,7 @@
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>UT1_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4815,11 +4715,7 @@
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>UT2_kidney</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -4949,11 +4845,7 @@
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>UT2_tumor_Center</t>
-        </is>
-      </c>
+      <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -5083,11 +4975,7 @@
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>UT2_tumor_Far</t>
-        </is>
-      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -5217,11 +5105,7 @@
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>UT2_tumor_Near</t>
-        </is>
-      </c>
+      <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
           <t>UT2</t>

</xml_diff>

<commit_message>
Update dev_stage, alignment, manner of death in dcp2T1
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1495,7 +1495,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -1625,7 +1629,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -1755,7 +1763,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -1885,7 +1897,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2015,7 +2031,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2145,7 +2165,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2275,7 +2299,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr"/>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M12" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2405,7 +2433,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2535,7 +2567,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr"/>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M14" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2665,7 +2701,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M15" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2795,7 +2835,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M16" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -2925,7 +2969,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3055,7 +3103,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M18" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3185,7 +3237,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M19" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3315,7 +3371,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3445,7 +3505,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M21" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3575,7 +3639,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr"/>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M22" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3705,7 +3773,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr"/>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M23" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3835,7 +3907,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr"/>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -3965,7 +4041,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M25" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4095,7 +4175,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr"/>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4225,7 +4309,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr"/>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4355,7 +4443,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr"/>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M28" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4485,7 +4577,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4615,7 +4711,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M30" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4745,7 +4845,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr"/>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M31" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -4875,7 +4979,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M32" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -5005,7 +5113,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr"/>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr">
         <is>
           <t>surgical donor</t>
@@ -5135,7 +5247,11 @@
           <t>NCBITaxon:9606</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr"/>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>not applicable</t>
+        </is>
+      </c>
       <c r="M34" t="inlineStr">
         <is>
           <t>surgical donor</t>

</xml_diff>

<commit_message>
Change default mapping for library_id_repository
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1480,11 +1480,7 @@
           <t>IpiNivo_Complete_PBMC_CS</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>PBMCs</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
@@ -1553,7 +1549,7 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806027</t>
+          <t>fastq_generation_SRR13806027, fastq_generation_SRR13806059</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
@@ -1614,11 +1610,7 @@
           <t>IpiNivo_Complete_kidney_CS</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
@@ -1687,7 +1679,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806028</t>
+          <t>fastq_generation_SRR13806028, fastq_generation_SRR13806060</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
@@ -1748,11 +1740,7 @@
           <t>IpiNivo_Complete_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
@@ -1821,7 +1809,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806031</t>
+          <t>fastq_generation_SRR13806031, fastq_generation_SRR13806063</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1882,11 +1870,7 @@
           <t>IpiNivo_Complete_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
@@ -1955,7 +1939,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806030</t>
+          <t>fastq_generation_SRR13806030, fastq_generation_SRR13806062</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
@@ -2016,11 +2000,7 @@
           <t>IpiNivo_Complete_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
@@ -2089,7 +2069,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806029</t>
+          <t>fastq_generation_SRR13806029, fastq_generation_SRR13806061</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
@@ -2150,11 +2130,7 @@
           <t>IpiNivo_Mixed_PBMC_CS</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>PBMCs</t>
-        </is>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
@@ -2223,7 +2199,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806032</t>
+          <t>fastq_generation_SRR13806032, fastq_generation_SRR13806064</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
@@ -2284,11 +2260,7 @@
           <t>IpiNivo_Mixed_kidney_CS</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
@@ -2357,7 +2329,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806033</t>
+          <t>fastq_generation_SRR13806033, fastq_generation_SRR13806065</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
@@ -2418,11 +2390,7 @@
           <t>IpiNivo_Mixed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
@@ -2491,7 +2459,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806037</t>
+          <t>fastq_generation_SRR13806037, fastq_generation_SRR13806069</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
@@ -2552,11 +2520,7 @@
           <t>IpiNivo_Mixed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
@@ -2625,7 +2589,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806036</t>
+          <t>fastq_generation_SRR13806036, fastq_generation_SRR13806067</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
@@ -2686,11 +2650,7 @@
           <t>IpiNivo_Mixed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
@@ -2759,7 +2719,7 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806034</t>
+          <t>fastq_generation_SRR13806034, fastq_generation_SRR13806066</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
@@ -2820,11 +2780,7 @@
           <t>IpiNivo_Resistant_PBMC_CS</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>PBMCs</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
@@ -2893,7 +2849,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806038</t>
+          <t>fastq_generation_SRR13806038, fastq_generation_SRR13806070</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
@@ -2954,11 +2910,7 @@
           <t>IpiNivo_Resistant_kidney_CS</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
@@ -3027,7 +2979,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806039</t>
+          <t>fastq_generation_SRR13806039, fastq_generation_SRR13806071</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
@@ -3088,11 +3040,7 @@
           <t>IpiNivo_Resistant_lymph_node_CS</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Cell suspension from lymph node</t>
-        </is>
-      </c>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
@@ -3161,7 +3109,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806040</t>
+          <t>fastq_generation_SRR13806040, fastq_generation_SRR13806072</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
@@ -3222,11 +3170,7 @@
           <t>IpiNivo_Resistant_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
@@ -3295,7 +3239,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806043</t>
+          <t>fastq_generation_SRR13806043, fastq_generation_SRR13806075</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr">
@@ -3356,11 +3300,7 @@
           <t>IpiNivo_Resistant_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
@@ -3429,7 +3369,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806042</t>
+          <t>fastq_generation_SRR13806042, fastq_generation_SRR13806074</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
@@ -3490,11 +3430,7 @@
           <t>IpiNivo_Resistant_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
@@ -3563,7 +3499,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806041</t>
+          <t>fastq_generation_SRR13806041, fastq_generation_SRR13806073</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
@@ -3624,11 +3560,7 @@
           <t>NivoExposed_PBMC_CS</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>PBMCs</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
@@ -3697,7 +3629,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806044</t>
+          <t>fastq_generation_SRR13806044, fastq_generation_SRR13806076</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
@@ -3758,11 +3690,7 @@
           <t>NivoExposed_kidney_CS</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
@@ -3831,7 +3759,7 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806045</t>
+          <t>fastq_generation_SRR13806045, fastq_generation_SRR13806077</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
@@ -3892,11 +3820,7 @@
           <t>NivoExposed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
@@ -3965,7 +3889,7 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806047</t>
+          <t>fastq_generation_SRR13806047, fastq_generation_SRR13806078</t>
         </is>
       </c>
       <c r="AC24" t="inlineStr">
@@ -4026,11 +3950,7 @@
           <t>NivoExposed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
@@ -4099,7 +4019,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806023</t>
+          <t>fastq_generation_SRR13806023, fastq_generation_SRR13806048</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
@@ -4160,11 +4080,7 @@
           <t>NivoExposed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
@@ -4233,7 +4149,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806024</t>
+          <t>fastq_generation_SRR13806024, fastq_generation_SRR13806049</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr">
@@ -4294,11 +4210,7 @@
           <t>UT1_kidney_CS</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
@@ -4367,7 +4279,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806054</t>
+          <t>fastq_generation_SRR13806054, fastq_generation_SRR13806057</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr">
@@ -4428,11 +4340,7 @@
           <t>UT1_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
@@ -4501,7 +4409,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806058</t>
+          <t>fastq_generation_SRR13806058, fastq_generation_SRR13806080</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr">
@@ -4562,11 +4470,7 @@
           <t>UT1_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
@@ -4635,7 +4539,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806055</t>
+          <t>fastq_generation_SRR13806055, fastq_generation_SRR13806068</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr">
@@ -4696,11 +4600,7 @@
           <t>UT1_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
@@ -4769,7 +4669,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806056</t>
+          <t>fastq_generation_SRR13806056, fastq_generation_SRR13806079</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr">
@@ -4830,11 +4730,7 @@
           <t>UT2_kidney_CS</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Cell suspension from normal kidney tissue</t>
-        </is>
-      </c>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
@@ -4903,7 +4799,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806025</t>
+          <t>fastq_generation_SRR13806025, fastq_generation_SRR13806050</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr">
@@ -4964,11 +4860,7 @@
           <t>UT2_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Center)</t>
-        </is>
-      </c>
+      <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
@@ -5037,7 +4929,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806046</t>
+          <t>fastq_generation_SRR13806046, fastq_generation_SRR13806053</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr">
@@ -5098,11 +4990,7 @@
           <t>UT2_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Far)</t>
-        </is>
-      </c>
+      <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
@@ -5171,7 +5059,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806035</t>
+          <t>fastq_generation_SRR13806035, fastq_generation_SRR13806052</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr">
@@ -5232,11 +5120,7 @@
           <t>UT2_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>Cell suspension from tumor tissue (Near)</t>
-        </is>
-      </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
@@ -5305,7 +5189,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806026</t>
+          <t>fastq_generation_SRR13806026, fastq_generation_SRR13806051</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr">

</xml_diff>

<commit_message>
Update tissue field with most detailed organ vs organ_part
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1522,7 +1522,11 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>blood</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1549,7 +1553,7 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806027, fastq_generation_SRR13806059</t>
+          <t>SRR13806027, SRR13806059</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
@@ -1559,7 +1563,7 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
@@ -1652,7 +1656,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1679,7 +1687,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806028, fastq_generation_SRR13806060</t>
+          <t>SRR13806028, SRR13806060</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
@@ -1689,7 +1697,7 @@
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
@@ -1782,7 +1790,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1809,7 +1821,7 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806031, fastq_generation_SRR13806063</t>
+          <t>SRR13806063</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1819,7 +1831,7 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -1912,7 +1924,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1939,7 +1955,7 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806030, fastq_generation_SRR13806062</t>
+          <t>SRR13806030, SRR13806062</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
@@ -1949,7 +1965,7 @@
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
@@ -2042,7 +2058,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2069,7 +2089,7 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806029, fastq_generation_SRR13806061</t>
+          <t>SRR13806061</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
@@ -2079,7 +2099,7 @@
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
@@ -2172,7 +2192,11 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>blood</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2199,7 +2223,7 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806032, fastq_generation_SRR13806064</t>
+          <t>SRR13806064</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
@@ -2209,7 +2233,7 @@
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2302,7 +2326,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2329,7 +2357,7 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806033, fastq_generation_SRR13806065</t>
+          <t>SRR13806065</t>
         </is>
       </c>
       <c r="AC12" t="inlineStr">
@@ -2339,7 +2367,7 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
@@ -2432,7 +2460,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2459,7 +2491,7 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806037, fastq_generation_SRR13806069</t>
+          <t>SRR13806069</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
@@ -2469,7 +2501,7 @@
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
@@ -2562,7 +2594,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T14" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2589,7 +2625,7 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806036, fastq_generation_SRR13806067</t>
+          <t>SRR13806067</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
@@ -2599,7 +2635,7 @@
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
@@ -2692,7 +2728,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2719,7 +2759,7 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806034, fastq_generation_SRR13806066</t>
+          <t>SRR13806066</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
@@ -2729,7 +2769,7 @@
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2822,7 +2862,11 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>blood</t>
+        </is>
+      </c>
       <c r="T16" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2849,7 +2893,7 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806038, fastq_generation_SRR13806070</t>
+          <t>SRR13806070</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
@@ -2859,7 +2903,7 @@
       </c>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
@@ -2952,7 +2996,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2979,7 +3027,7 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806039, fastq_generation_SRR13806071</t>
+          <t>SRR13806071</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
@@ -2989,7 +3037,7 @@
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE17" t="inlineStr">
@@ -3082,7 +3130,11 @@
           <t>UBERON:0000029</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>lymph node</t>
+        </is>
+      </c>
       <c r="T18" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3109,7 +3161,7 @@
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806040, fastq_generation_SRR13806072</t>
+          <t>SRR13806072</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
@@ -3119,7 +3171,7 @@
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE18" t="inlineStr">
@@ -3212,7 +3264,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T19" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3239,7 +3295,7 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806043, fastq_generation_SRR13806075</t>
+          <t>SRR13806075</t>
         </is>
       </c>
       <c r="AC19" t="inlineStr">
@@ -3249,7 +3305,7 @@
       </c>
       <c r="AD19" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE19" t="inlineStr">
@@ -3342,7 +3398,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T20" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3369,7 +3429,7 @@
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806042, fastq_generation_SRR13806074</t>
+          <t>SRR13806074</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
@@ -3379,7 +3439,7 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
@@ -3472,7 +3532,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T21" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3499,7 +3563,7 @@
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806041, fastq_generation_SRR13806073</t>
+          <t>SRR13806073</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
@@ -3509,7 +3573,7 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
@@ -3602,7 +3666,11 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>blood</t>
+        </is>
+      </c>
       <c r="T22" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3629,7 +3697,7 @@
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806044, fastq_generation_SRR13806076</t>
+          <t>SRR13806076</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
@@ -3639,7 +3707,7 @@
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
@@ -3732,7 +3800,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T23" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3759,7 +3831,7 @@
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806045, fastq_generation_SRR13806077</t>
+          <t>SRR13806077</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
@@ -3769,7 +3841,7 @@
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
@@ -3862,7 +3934,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr"/>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T24" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3889,7 +3965,7 @@
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806047, fastq_generation_SRR13806078</t>
+          <t>SRR13806078</t>
         </is>
       </c>
       <c r="AC24" t="inlineStr">
@@ -3899,7 +3975,7 @@
       </c>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
@@ -3992,7 +4068,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T25" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4019,7 +4099,7 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806023, fastq_generation_SRR13806048</t>
+          <t>SRR13806023</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
@@ -4029,7 +4109,7 @@
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
@@ -4122,7 +4202,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T26" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4149,7 +4233,7 @@
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806024, fastq_generation_SRR13806049</t>
+          <t>SRR13806024</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr">
@@ -4159,7 +4243,7 @@
       </c>
       <c r="AD26" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE26" t="inlineStr">
@@ -4252,7 +4336,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr"/>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T27" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4279,7 +4367,7 @@
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806054, fastq_generation_SRR13806057</t>
+          <t>SRR13806057</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr">
@@ -4289,7 +4377,7 @@
       </c>
       <c r="AD27" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE27" t="inlineStr">
@@ -4382,7 +4470,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr"/>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T28" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4409,7 +4501,7 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806058, fastq_generation_SRR13806080</t>
+          <t>SRR13806080</t>
         </is>
       </c>
       <c r="AC28" t="inlineStr">
@@ -4419,7 +4511,7 @@
       </c>
       <c r="AD28" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE28" t="inlineStr">
@@ -4512,7 +4604,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T29" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4539,7 +4635,7 @@
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806055, fastq_generation_SRR13806068</t>
+          <t>SRR13806068</t>
         </is>
       </c>
       <c r="AC29" t="inlineStr">
@@ -4549,7 +4645,7 @@
       </c>
       <c r="AD29" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE29" t="inlineStr">
@@ -4642,7 +4738,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr"/>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T30" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4669,7 +4769,7 @@
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806056, fastq_generation_SRR13806079</t>
+          <t>SRR13806079</t>
         </is>
       </c>
       <c r="AC30" t="inlineStr">
@@ -4679,7 +4779,7 @@
       </c>
       <c r="AD30" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE30" t="inlineStr">
@@ -4772,7 +4872,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr"/>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T31" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4799,7 +4903,7 @@
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806025, fastq_generation_SRR13806050</t>
+          <t>SRR13806025</t>
         </is>
       </c>
       <c r="AC31" t="inlineStr">
@@ -4809,7 +4913,7 @@
       </c>
       <c r="AD31" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE31" t="inlineStr">
@@ -4902,7 +5006,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T32" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4929,7 +5037,7 @@
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806046, fastq_generation_SRR13806053</t>
+          <t>SRR13806046</t>
         </is>
       </c>
       <c r="AC32" t="inlineStr">
@@ -4939,7 +5047,7 @@
       </c>
       <c r="AD32" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE32" t="inlineStr">
@@ -5032,7 +5140,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr"/>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T33" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -5059,7 +5171,7 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806035, fastq_generation_SRR13806052</t>
+          <t>SRR13806035</t>
         </is>
       </c>
       <c r="AC33" t="inlineStr">
@@ -5069,7 +5181,7 @@
       </c>
       <c r="AD33" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE33" t="inlineStr">
@@ -5162,7 +5274,11 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr"/>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>kidney</t>
+        </is>
+      </c>
       <c r="T34" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -5189,7 +5305,7 @@
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr">
         <is>
-          <t>fastq_generation_SRR13806026, fastq_generation_SRR13806051</t>
+          <t>SRR13806026</t>
         </is>
       </c>
       <c r="AC34" t="inlineStr">
@@ -5199,7 +5315,7 @@
       </c>
       <c r="AD34" t="inlineStr">
         <is>
-          <t>EFO:0008565</t>
+          <t>Illumina HiSeq 2500</t>
         </is>
       </c>
       <c r="AE34" t="inlineStr">

</xml_diff>

<commit_message>
Add tissue_free_text only if different from label
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1522,11 +1522,7 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>blood</t>
-        </is>
-      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1656,11 +1652,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1790,11 +1782,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -1924,11 +1912,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2058,11 +2042,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2192,11 +2172,7 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>blood</t>
-        </is>
-      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2326,11 +2302,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2460,11 +2432,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2594,11 +2562,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2728,11 +2692,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2862,11 +2822,7 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>blood</t>
-        </is>
-      </c>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -2996,11 +2952,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3130,11 +3082,7 @@
           <t>UBERON:0000029</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>lymph node</t>
-        </is>
-      </c>
+      <c r="S18" t="inlineStr"/>
       <c r="T18" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3264,11 +3212,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S19" t="inlineStr"/>
       <c r="T19" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3398,11 +3342,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S20" t="inlineStr"/>
       <c r="T20" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3532,11 +3472,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S21" t="inlineStr"/>
       <c r="T21" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3666,11 +3602,7 @@
           <t>UBERON:0000178</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>blood</t>
-        </is>
-      </c>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3800,11 +3732,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -3934,11 +3862,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S24" t="inlineStr"/>
       <c r="T24" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4068,11 +3992,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S25" t="inlineStr"/>
       <c r="T25" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4202,11 +4122,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4336,11 +4252,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S27" t="inlineStr"/>
       <c r="T27" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4470,11 +4382,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4604,11 +4512,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S29" t="inlineStr"/>
       <c r="T29" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4738,11 +4642,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S30" t="inlineStr"/>
       <c r="T30" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -4872,11 +4772,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S31" t="inlineStr"/>
       <c r="T31" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -5006,11 +4902,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S32" t="inlineStr"/>
       <c r="T32" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -5140,11 +5032,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S33" t="inlineStr"/>
       <c r="T33" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>
@@ -5274,11 +5162,7 @@
           <t>UBERON:0002113</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>kidney</t>
-        </is>
-      </c>
+      <c r="S34" t="inlineStr"/>
       <c r="T34" t="inlineStr">
         <is>
           <t>frozen in liquid nitrogen</t>

</xml_diff>

<commit_message>
Add updated output files
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1465,7 +1465,11 @@
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_PBMC</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1595,7 +1599,11 @@
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_kidney</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1725,7 +1733,11 @@
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Center</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1855,7 +1867,11 @@
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Far</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -1985,7 +2001,11 @@
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IpiNivo_Complete_tumor_Near</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>IpiNivo_Complete</t>
@@ -2115,7 +2135,11 @@
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_PBMC</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2245,7 +2269,11 @@
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_kidney</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2375,7 +2403,11 @@
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Center</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2505,7 +2537,11 @@
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Far</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2635,7 +2671,11 @@
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IpiNivo_Mixed_tumor_Near</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>IpiNivo_Mixed</t>
@@ -2765,7 +2805,11 @@
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_PBMC</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -2895,7 +2939,11 @@
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_kidney</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3025,7 +3073,11 @@
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_lymph_node</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3155,7 +3207,11 @@
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Center</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3285,7 +3341,11 @@
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Far</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3415,7 +3475,11 @@
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>IpiNivo_Resistant_tumor_Near</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>IpiNivo_Resistant</t>
@@ -3545,7 +3609,11 @@
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NivoExposed_PBMC</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3675,7 +3743,11 @@
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NivoExposed_kidney</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3805,7 +3877,11 @@
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Center</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -3935,7 +4011,11 @@
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Far</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4065,7 +4145,11 @@
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NivoExposed_tumor_Near</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>NivoExposed</t>
@@ -4195,7 +4279,11 @@
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>UT1_kidney</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4325,7 +4413,11 @@
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Center</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4455,7 +4547,11 @@
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Far</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4585,7 +4681,11 @@
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>UT1_tumor_Near</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>UT1</t>
@@ -4715,7 +4815,11 @@
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>UT2_kidney</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -4845,7 +4949,11 @@
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Center</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -4975,7 +5083,11 @@
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Far</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>UT2</t>
@@ -5105,7 +5217,11 @@
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>UT2_tumor_Near</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>UT2</t>

</xml_diff>

<commit_message>
Add library_id_repository from insdc_experiment_accession
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1484,7 +1484,11 @@
           <t>IpiNivo_Complete_PBMC_CS</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>SRX10189013, SRX10188981</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
@@ -1618,7 +1622,11 @@
           <t>IpiNivo_Complete_kidney_CS</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>SRX10189012, SRX10188980</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
@@ -1752,7 +1760,11 @@
           <t>IpiNivo_Complete_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>SRX10188977</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr">
         <is>
@@ -1886,7 +1898,11 @@
           <t>IpiNivo_Complete_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>SRX10189010, SRX10188978</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr">
         <is>
@@ -2020,7 +2036,11 @@
           <t>IpiNivo_Complete_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>SRX10188979</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
@@ -2154,7 +2174,11 @@
           <t>IpiNivo_Mixed_PBMC_CS</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>SRX10188976</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
@@ -2288,7 +2312,11 @@
           <t>IpiNivo_Mixed_kidney_CS</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>SRX10188975</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
@@ -2422,7 +2450,11 @@
           <t>IpiNivo_Mixed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>SRX10188971</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
@@ -2556,7 +2588,11 @@
           <t>IpiNivo_Mixed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>SRX10188973</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
@@ -2690,7 +2726,11 @@
           <t>IpiNivo_Mixed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>SRX10188974</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
@@ -2824,7 +2864,11 @@
           <t>IpiNivo_Resistant_PBMC_CS</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>SRX10188970</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
@@ -2958,7 +3002,11 @@
           <t>IpiNivo_Resistant_kidney_CS</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>SRX10188969</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
@@ -3092,7 +3140,11 @@
           <t>IpiNivo_Resistant_lymph_node_CS</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>SRX10188968</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
@@ -3226,7 +3278,11 @@
           <t>IpiNivo_Resistant_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>SRX10188965</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
@@ -3360,7 +3416,11 @@
           <t>IpiNivo_Resistant_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SRX10188966</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
@@ -3494,7 +3554,11 @@
           <t>IpiNivo_Resistant_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>SRX10188967</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
@@ -3628,7 +3692,11 @@
           <t>NivoExposed_PBMC_CS</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>SRX10188964</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
         <is>
@@ -3762,7 +3830,11 @@
           <t>NivoExposed_kidney_CS</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>SRX10188963</t>
+        </is>
+      </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
@@ -3896,7 +3968,11 @@
           <t>NivoExposed_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>SRX10188962</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
@@ -4030,7 +4106,11 @@
           <t>NivoExposed_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>SRX10189017</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
@@ -4164,7 +4244,11 @@
           <t>NivoExposed_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>SRX10189016</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
@@ -4298,7 +4382,11 @@
           <t>UT1_kidney_CS</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>SRX10188983</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
@@ -4432,7 +4520,11 @@
           <t>UT1_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>SRX10188960</t>
+        </is>
+      </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
@@ -4566,7 +4658,11 @@
           <t>UT1_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>SRX10188972</t>
+        </is>
+      </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
@@ -4700,7 +4796,11 @@
           <t>UT1_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>SRX10188961</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
@@ -4834,7 +4934,11 @@
           <t>UT2_kidney_CS</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>SRX10189015</t>
+        </is>
+      </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
@@ -4968,7 +5072,11 @@
           <t>UT2_tumor_Center_CS</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>SRX10188994</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
@@ -5102,7 +5210,11 @@
           <t>UT2_tumor_Far_CS</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>SRX10189005</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
@@ -5236,7 +5348,11 @@
           <t>UT2_tumor_Near_CS</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>SRX10189014</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add exception if donor age is not provided
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1595,7 +1595,7 @@
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>63</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr"/>
@@ -1733,7 +1733,7 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>63</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr"/>
@@ -1871,7 +1871,7 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>63</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr"/>
@@ -2009,7 +2009,7 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>63</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr"/>
@@ -2147,7 +2147,7 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>63</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>64</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr"/>
@@ -2423,7 +2423,7 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>64</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr"/>
@@ -2561,7 +2561,7 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>64</t>
         </is>
       </c>
       <c r="AM13" t="inlineStr"/>
@@ -2699,7 +2699,7 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>64</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr"/>
@@ -2837,7 +2837,7 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>64</t>
         </is>
       </c>
       <c r="AM15" t="inlineStr"/>
@@ -2975,7 +2975,7 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM16" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM17" t="inlineStr"/>
@@ -3251,7 +3251,7 @@
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM18" t="inlineStr"/>
@@ -3389,7 +3389,7 @@
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM19" t="inlineStr"/>
@@ -3527,7 +3527,7 @@
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM20" t="inlineStr"/>
@@ -3665,7 +3665,7 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>50</t>
         </is>
       </c>
       <c r="AM21" t="inlineStr"/>
@@ -3803,7 +3803,7 @@
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>54</t>
         </is>
       </c>
       <c r="AM22" t="inlineStr"/>
@@ -3941,7 +3941,7 @@
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>54</t>
         </is>
       </c>
       <c r="AM23" t="inlineStr"/>
@@ -4079,7 +4079,7 @@
       <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>54</t>
         </is>
       </c>
       <c r="AM24" t="inlineStr"/>
@@ -4217,7 +4217,7 @@
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>54</t>
         </is>
       </c>
       <c r="AM25" t="inlineStr"/>
@@ -4355,7 +4355,7 @@
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>54</t>
         </is>
       </c>
       <c r="AM26" t="inlineStr"/>
@@ -4493,7 +4493,7 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>69</t>
         </is>
       </c>
       <c r="AM27" t="inlineStr"/>
@@ -4631,7 +4631,7 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>69</t>
         </is>
       </c>
       <c r="AM28" t="inlineStr"/>
@@ -4769,7 +4769,7 @@
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>69</t>
         </is>
       </c>
       <c r="AM29" t="inlineStr"/>
@@ -4907,7 +4907,7 @@
       <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="inlineStr">
         <is>
-          <t>HsapDv:0000241</t>
+          <t>69</t>
         </is>
       </c>
       <c r="AM30" t="inlineStr"/>
@@ -5045,7 +5045,7 @@
       <c r="AK31" t="inlineStr"/>
       <c r="AL31" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>57</t>
         </is>
       </c>
       <c r="AM31" t="inlineStr"/>
@@ -5183,7 +5183,7 @@
       <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>57</t>
         </is>
       </c>
       <c r="AM32" t="inlineStr"/>
@@ -5321,7 +5321,7 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>57</t>
         </is>
       </c>
       <c r="AM33" t="inlineStr"/>
@@ -5459,7 +5459,7 @@
       <c r="AK34" t="inlineStr"/>
       <c r="AL34" t="inlineStr">
         <is>
-          <t>HsapDv:0000240</t>
+          <t>57</t>
         </is>
       </c>
       <c r="AM34" t="inlineStr"/>

</xml_diff>

<commit_message>
Add button to select filename, filled percentage counter
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1595,7 +1595,7 @@
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr"/>
@@ -1733,7 +1733,7 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr"/>
@@ -1871,7 +1871,7 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr"/>
@@ -2009,7 +2009,7 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr"/>
@@ -2147,7 +2147,7 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr"/>
@@ -2423,7 +2423,7 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr"/>
@@ -2561,7 +2561,7 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM13" t="inlineStr"/>
@@ -2699,7 +2699,7 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM14" t="inlineStr"/>
@@ -2837,7 +2837,7 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM15" t="inlineStr"/>
@@ -2975,7 +2975,7 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM16" t="inlineStr"/>
@@ -3113,7 +3113,7 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM17" t="inlineStr"/>
@@ -3251,7 +3251,7 @@
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM18" t="inlineStr"/>
@@ -3389,7 +3389,7 @@
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM19" t="inlineStr"/>
@@ -3527,7 +3527,7 @@
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM20" t="inlineStr"/>
@@ -3665,7 +3665,7 @@
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM21" t="inlineStr"/>
@@ -3803,7 +3803,7 @@
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM22" t="inlineStr"/>
@@ -3941,7 +3941,7 @@
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM23" t="inlineStr"/>
@@ -4079,7 +4079,7 @@
       <c r="AK24" t="inlineStr"/>
       <c r="AL24" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM24" t="inlineStr"/>
@@ -4217,7 +4217,7 @@
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM25" t="inlineStr"/>
@@ -4355,7 +4355,7 @@
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM26" t="inlineStr"/>
@@ -4493,7 +4493,7 @@
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM27" t="inlineStr"/>
@@ -4631,7 +4631,7 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM28" t="inlineStr"/>
@@ -4769,7 +4769,7 @@
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM29" t="inlineStr"/>
@@ -4907,7 +4907,7 @@
       <c r="AK30" t="inlineStr"/>
       <c r="AL30" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>HsapDv:0000241</t>
         </is>
       </c>
       <c r="AM30" t="inlineStr"/>
@@ -5045,7 +5045,7 @@
       <c r="AK31" t="inlineStr"/>
       <c r="AL31" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM31" t="inlineStr"/>
@@ -5183,7 +5183,7 @@
       <c r="AK32" t="inlineStr"/>
       <c r="AL32" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM32" t="inlineStr"/>
@@ -5321,7 +5321,7 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM33" t="inlineStr"/>
@@ -5459,7 +5459,7 @@
       <c r="AK34" t="inlineStr"/>
       <c r="AL34" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>HsapDv:0000240</t>
         </is>
       </c>
       <c r="AM34" t="inlineStr"/>

</xml_diff>

<commit_message>
Update to file agnostic for alignment and preservation
</commit_message>
<xml_diff>
--- a/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
+++ b/tier1_output/ImmuneLandscapeccRCC_metadata_30-01-2023_Tier1.xlsx
@@ -1583,7 +1583,7 @@
       <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr"/>
@@ -1721,7 +1721,7 @@
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr"/>
@@ -1859,7 +1859,7 @@
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr"/>
@@ -1997,7 +1997,7 @@
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr"/>
@@ -2135,7 +2135,7 @@
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr"/>
@@ -2273,7 +2273,7 @@
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr"/>
@@ -2411,7 +2411,7 @@
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI12" t="inlineStr"/>
@@ -2549,7 +2549,7 @@
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr"/>
@@ -2687,7 +2687,7 @@
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI14" t="inlineStr"/>
@@ -2825,7 +2825,7 @@
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr"/>
@@ -2963,7 +2963,7 @@
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI16" t="inlineStr"/>
@@ -3101,7 +3101,7 @@
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI17" t="inlineStr"/>
@@ -3239,7 +3239,7 @@
       <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI18" t="inlineStr"/>
@@ -3377,7 +3377,7 @@
       <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI19" t="inlineStr"/>
@@ -3515,7 +3515,7 @@
       <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI20" t="inlineStr"/>
@@ -3653,7 +3653,7 @@
       <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI21" t="inlineStr"/>
@@ -3791,7 +3791,7 @@
       <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI22" t="inlineStr"/>
@@ -3929,7 +3929,7 @@
       <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI23" t="inlineStr"/>
@@ -4067,7 +4067,7 @@
       <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI24" t="inlineStr"/>
@@ -4205,7 +4205,7 @@
       <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI25" t="inlineStr"/>
@@ -4343,7 +4343,7 @@
       <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI26" t="inlineStr"/>
@@ -4481,7 +4481,7 @@
       <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI27" t="inlineStr"/>
@@ -4619,7 +4619,7 @@
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI28" t="inlineStr"/>
@@ -4757,7 +4757,7 @@
       <c r="AG29" t="inlineStr"/>
       <c r="AH29" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI29" t="inlineStr"/>
@@ -4895,7 +4895,7 @@
       <c r="AG30" t="inlineStr"/>
       <c r="AH30" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI30" t="inlineStr"/>
@@ -5033,7 +5033,7 @@
       <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI31" t="inlineStr"/>
@@ -5171,7 +5171,7 @@
       <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI32" t="inlineStr"/>
@@ -5309,7 +5309,7 @@
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI33" t="inlineStr"/>
@@ -5447,7 +5447,7 @@
       <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="inlineStr">
         <is>
-          <t>Cellranger v3.0.2</t>
+          <t>Cellranger v3.0.1</t>
         </is>
       </c>
       <c r="AI34" t="inlineStr"/>

</xml_diff>